<commit_message>
optimizing and checking the algo and adding a Chi2 test
</commit_message>
<xml_diff>
--- a/data/realpage_market_cr.xlsx
+++ b/data/realpage_market_cr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\inflation_cr_expansion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB08CD49-D6F6-4966-8B4F-EDDE16419D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FD7338-6546-4A44-9351-AA00243280E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32175" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEOGRAPHIES" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
   <si>
     <t>Geography Name</t>
   </si>
@@ -406,6 +406,36 @@
   </si>
   <si>
     <t>Y2021Q3</t>
+  </si>
+  <si>
+    <t>San Antonio-New Braunfels, TX</t>
+  </si>
+  <si>
+    <t>San Jose-Sunnyvale-Santa Clara, CA</t>
+  </si>
+  <si>
+    <t>Columbus, OH</t>
+  </si>
+  <si>
+    <t>Indianapolis-Carmel-Anderson, IN</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
+  </si>
+  <si>
+    <t>Jacksonville, FL</t>
+  </si>
+  <si>
+    <t>Jacksonville</t>
+  </si>
+  <si>
+    <t>Columbus</t>
+  </si>
+  <si>
+    <t>SanJose</t>
   </si>
 </sst>
 </file>
@@ -467,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,6 +507,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,7 +824,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CI20"/>
+  <dimension ref="A1:CI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -801,7 +833,7 @@
     <col min="3" max="23" width="16" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1058,7 +1090,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1314,14 +1346,8 @@
       <c r="CG2">
         <v>4.7870708050830602E-2</v>
       </c>
-      <c r="CH2" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1577,14 +1603,8 @@
       <c r="CG3">
         <v>5.14074607471968E-2</v>
       </c>
-      <c r="CH3" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1840,14 +1860,8 @@
       <c r="CG4">
         <v>4.4068083643351998E-2</v>
       </c>
-      <c r="CH4" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2103,14 +2117,8 @@
       <c r="CG5">
         <v>5.0581629697618702E-2</v>
       </c>
-      <c r="CH5" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2366,14 +2374,8 @@
       <c r="CG6">
         <v>4.6145597661125103E-2</v>
       </c>
-      <c r="CH6" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI6" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2629,14 +2631,8 @@
       <c r="CG7">
         <v>4.35329961887874E-2</v>
       </c>
-      <c r="CH7" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI7" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2892,14 +2888,8 @@
       <c r="CG8">
         <v>4.92741828603213E-2</v>
       </c>
-      <c r="CH8" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI8" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -3155,14 +3145,8 @@
       <c r="CG9">
         <v>4.3067592293483198E-2</v>
       </c>
-      <c r="CH9" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI9" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -3418,14 +3402,8 @@
       <c r="CG10">
         <v>4.6944635306451599E-2</v>
       </c>
-      <c r="CH10" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI10" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -3681,14 +3659,8 @@
       <c r="CG11">
         <v>4.7550908072163903E-2</v>
       </c>
-      <c r="CH11" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI11" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -3944,14 +3916,8 @@
       <c r="CG12">
         <v>4.6755518098505998E-2</v>
       </c>
-      <c r="CH12" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI12" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -4207,14 +4173,8 @@
       <c r="CG13">
         <v>4.9790917210938701E-2</v>
       </c>
-      <c r="CH13" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI13" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4470,14 +4430,8 @@
       <c r="CG14">
         <v>4.3513993359494199E-2</v>
       </c>
-      <c r="CH14" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI14" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4733,14 +4687,8 @@
       <c r="CG15">
         <v>4.2619840349245298E-2</v>
       </c>
-      <c r="CH15" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI15" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -4995,12 +4943,6 @@
       </c>
       <c r="CG16">
         <v>3.9655819377456103E-2</v>
-      </c>
-      <c r="CH16" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:87" x14ac:dyDescent="0.25">
@@ -5259,12 +5201,6 @@
       <c r="CG17">
         <v>4.1980557011838497E-2</v>
       </c>
-      <c r="CH17" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI17" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="18" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5522,12 +5458,6 @@
       <c r="CG18">
         <v>5.3355687826240103E-2</v>
       </c>
-      <c r="CH18" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI18" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="19" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -5785,12 +5715,6 @@
       <c r="CG19">
         <v>4.7860483840902399E-2</v>
       </c>
-      <c r="CH19" t="s">
-        <v>23</v>
-      </c>
-      <c r="CI19" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="20" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -6048,11 +5972,1296 @@
       <c r="CG20">
         <v>4.6838490123922903E-2</v>
       </c>
-      <c r="CH20" t="s">
+    </row>
+    <row r="21" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="3">
+        <v>8.9058275058275099E-2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>8.0741356255969399E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>8.0539662821650398E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8.1976092333058498E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>7.8100765306122394E-2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>8.5555028462998103E-2</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8.6423014354067004E-2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>8.6461882716049404E-2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>8.4821681810083704E-2</v>
+      </c>
+      <c r="L21" s="3">
+        <v>8.4140504334121402E-2</v>
+      </c>
+      <c r="M21" s="3">
+        <v>8.1997807843808904E-2</v>
+      </c>
+      <c r="N21" s="3">
+        <v>8.0773477812177502E-2</v>
+      </c>
+      <c r="O21" s="3">
+        <v>7.7533163501621094E-2</v>
+      </c>
+      <c r="P21" s="3">
+        <v>7.7956710872920804E-2</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>7.7885334593328595E-2</v>
+      </c>
+      <c r="R21" s="3">
+        <v>7.2804009827804106E-2</v>
+      </c>
+      <c r="S21" s="3">
+        <v>7.5668146553662996E-2</v>
+      </c>
+      <c r="T21" s="3">
+        <v>7.2781293706293701E-2</v>
+      </c>
+      <c r="U21" s="3">
+        <v>7.1924215322308499E-2</v>
+      </c>
+      <c r="V21" s="3">
+        <v>7.6305209374584196E-2</v>
+      </c>
+      <c r="W21" s="3">
+        <v>7.4627723435749402E-2</v>
+      </c>
+      <c r="X21" s="6">
+        <v>7.5513300355720597E-2</v>
+      </c>
+      <c r="Y21" s="6">
+        <v>7.3262452357941807E-2</v>
+      </c>
+      <c r="Z21" s="6">
+        <v>6.5612826590505699E-2</v>
+      </c>
+      <c r="AA21" s="6">
+        <v>6.6789691495512796E-2</v>
+      </c>
+      <c r="AB21" s="6">
+        <v>6.7042577499016598E-2</v>
+      </c>
+      <c r="AC21" s="6">
+        <v>6.7522001715486099E-2</v>
+      </c>
+      <c r="AD21" s="6">
+        <v>7.1674609922927998E-2</v>
+      </c>
+      <c r="AE21" s="6">
+        <v>7.1783531685492605E-2</v>
+      </c>
+      <c r="AF21" s="6">
+        <v>7.4914251465903706E-2</v>
+      </c>
+      <c r="AG21" s="6">
+        <v>7.7251316595223496E-2</v>
+      </c>
+      <c r="AH21" s="6">
+        <v>7.1972986900082594E-2</v>
+      </c>
+      <c r="AI21" s="6">
+        <v>7.0732383844092597E-2</v>
+      </c>
+      <c r="AJ21" s="6">
+        <v>7.0549768721311495E-2</v>
+      </c>
+      <c r="AK21" s="6">
+        <v>6.5660070371428597E-2</v>
+      </c>
+      <c r="AL21" s="6">
+        <v>6.8136462765799294E-2</v>
+      </c>
+      <c r="AM21" s="6">
+        <v>6.8136462765799294E-2</v>
+      </c>
+      <c r="AN21" s="6">
+        <v>6.7547378454828694E-2</v>
+      </c>
+      <c r="AO21" s="6">
+        <v>6.8300806823340096E-2</v>
+      </c>
+      <c r="AP21" s="6">
+        <v>6.6593458214626394E-2</v>
+      </c>
+      <c r="AQ21" s="6">
+        <v>6.8888435912693502E-2</v>
+      </c>
+      <c r="AR21" s="6">
+        <v>6.5451999535616104E-2</v>
+      </c>
+      <c r="AS21" s="6">
+        <v>6.1725284990439798E-2</v>
+      </c>
+      <c r="AT21" s="6">
+        <v>6.1937714226386102E-2</v>
+      </c>
+      <c r="AU21" s="6">
+        <v>5.9879650659762598E-2</v>
+      </c>
+      <c r="AV21" s="6">
+        <v>6.2516449701720794E-2</v>
+      </c>
+      <c r="AW21" s="6">
+        <v>6.4691214702214103E-2</v>
+      </c>
+      <c r="AX21" s="6">
+        <v>6.4211930266140804E-2</v>
+      </c>
+      <c r="AY21" s="6">
+        <v>6.3826327305090802E-2</v>
+      </c>
+      <c r="AZ21" s="6">
+        <v>6.3440805390431898E-2</v>
+      </c>
+      <c r="BA21" s="6">
+        <v>6.3389160230746602E-2</v>
+      </c>
+      <c r="BB21" s="6">
+        <v>6.1045076979669897E-2</v>
+      </c>
+      <c r="BC21" s="6">
+        <v>6.0257228131667097E-2</v>
+      </c>
+      <c r="BD21" s="6">
+        <v>5.8570843436090203E-2</v>
+      </c>
+      <c r="BE21" s="6">
+        <v>5.8904644857164103E-2</v>
+      </c>
+      <c r="BF21" s="6">
+        <v>5.92780511170087E-2</v>
+      </c>
+      <c r="BG21" s="6">
+        <v>5.8360071834181397E-2</v>
+      </c>
+      <c r="BH21" s="6">
+        <v>5.8537428336514603E-2</v>
+      </c>
+      <c r="BI21" s="6">
+        <v>5.8700220779099303E-2</v>
+      </c>
+      <c r="BJ21" s="6">
+        <v>5.9211996854931698E-2</v>
+      </c>
+      <c r="BK21" s="6">
+        <v>5.97593436893568E-2</v>
+      </c>
+      <c r="BL21" s="6">
+        <v>5.87255594144298E-2</v>
+      </c>
+      <c r="BM21" s="6">
+        <v>5.7846552764668997E-2</v>
+      </c>
+      <c r="BN21" s="6">
+        <v>5.74467499792123E-2</v>
+      </c>
+      <c r="BO21" s="6">
+        <v>5.7487644520446898E-2</v>
+      </c>
+      <c r="BP21" s="6">
+        <v>5.81316172998095E-2</v>
+      </c>
+      <c r="BQ21" s="6">
+        <v>5.70656399622037E-2</v>
+      </c>
+      <c r="BR21" s="6">
+        <v>5.6155174283874301E-2</v>
+      </c>
+      <c r="BS21" s="6">
+        <v>5.5936081349802103E-2</v>
+      </c>
+      <c r="BT21" s="6">
+        <v>5.5615049406390102E-2</v>
+      </c>
+      <c r="BU21" s="6">
+        <v>5.6178859941395203E-2</v>
+      </c>
+      <c r="BV21" s="6">
+        <v>5.6085846825975602E-2</v>
+      </c>
+      <c r="BW21" s="6">
+        <v>5.5166768046089998E-2</v>
+      </c>
+      <c r="BX21" s="6">
+        <v>5.4950060932386302E-2</v>
+      </c>
+      <c r="BY21" s="6">
+        <v>5.4312965413887498E-2</v>
+      </c>
+      <c r="BZ21" s="6">
+        <v>5.3598585989643101E-2</v>
+      </c>
+      <c r="CA21" s="6">
+        <v>5.3321043642432397E-2</v>
+      </c>
+      <c r="CB21" s="6">
+        <v>5.2531654903979798E-2</v>
+      </c>
+      <c r="CC21" s="6">
+        <v>5.0979075825516203E-2</v>
+      </c>
+      <c r="CD21" s="6">
+        <v>4.95330529376811E-2</v>
+      </c>
+      <c r="CE21" s="6">
+        <v>4.8802868119752998E-2</v>
+      </c>
+      <c r="CF21" s="6">
+        <v>4.81787180740142E-2</v>
+      </c>
+      <c r="CG21" s="6">
+        <v>4.8100262187196902E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="CI20" t="s">
+      <c r="D22" s="3">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8.8430232558139504E-2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8.8288498402555898E-2</v>
+      </c>
+      <c r="G22" s="3">
+        <v>8.80185701830863E-2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>7.7888143382352906E-2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>7.8847770398481995E-2</v>
+      </c>
+      <c r="J22" s="3">
+        <v>7.8856223776223797E-2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>7.9065267459138194E-2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>7.8584501172180202E-2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>7.7290037493304806E-2</v>
+      </c>
+      <c r="N22" s="3">
+        <v>7.6163803519831902E-2</v>
+      </c>
+      <c r="O22" s="3">
+        <v>7.6029494927518398E-2</v>
+      </c>
+      <c r="P22" s="3">
+        <v>7.0615154835737506E-2</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>6.5137755059260602E-2</v>
+      </c>
+      <c r="R22" s="3">
+        <v>6.4818904713003694E-2</v>
+      </c>
+      <c r="S22" s="3">
+        <v>6.4928864986354196E-2</v>
+      </c>
+      <c r="T22" s="3">
+        <v>6.6079415326068106E-2</v>
+      </c>
+      <c r="U22" s="3">
+        <v>6.8487157894736805E-2</v>
+      </c>
+      <c r="V22" s="3">
+        <v>6.6983843036109103E-2</v>
+      </c>
+      <c r="W22" s="3">
+        <v>6.6213716138878304E-2</v>
+      </c>
+      <c r="X22" s="6">
+        <v>6.6787347427926594E-2</v>
+      </c>
+      <c r="Y22" s="6">
+        <v>6.9928099253710893E-2</v>
+      </c>
+      <c r="Z22" s="6">
+        <v>7.2800522979539095E-2</v>
+      </c>
+      <c r="AA22" s="6">
+        <v>7.4413769634318505E-2</v>
+      </c>
+      <c r="AB22" s="6">
+        <v>7.0083210997888098E-2</v>
+      </c>
+      <c r="AC22" s="6">
+        <v>6.8670025509546803E-2</v>
+      </c>
+      <c r="AD22" s="6">
+        <v>6.7288987971764705E-2</v>
+      </c>
+      <c r="AE22" s="6">
+        <v>6.4829736818785996E-2</v>
+      </c>
+      <c r="AF22" s="6">
+        <v>7.1669607734806601E-2</v>
+      </c>
+      <c r="AG22" s="6">
+        <v>7.3977116704805501E-2</v>
+      </c>
+      <c r="AH22" s="6">
+        <v>8.0456182472989204E-2</v>
+      </c>
+      <c r="AI22" s="6">
+        <v>8.66822202948829E-2</v>
+      </c>
+      <c r="AJ22" s="6">
+        <v>8.3708025776215597E-2</v>
+      </c>
+      <c r="AK22" s="6">
+        <v>8.4484864165588605E-2</v>
+      </c>
+      <c r="AL22" s="6">
+        <v>8.0320403022670003E-2</v>
+      </c>
+      <c r="AM22" s="6">
+        <v>7.2206640106241698E-2</v>
+      </c>
+      <c r="AN22" s="6">
+        <v>6.5797048611111103E-2</v>
+      </c>
+      <c r="AO22" s="6">
+        <v>6.6272976334951494E-2</v>
+      </c>
+      <c r="AP22" s="6">
+        <v>6.5636396874872799E-2</v>
+      </c>
+      <c r="AQ22" s="6">
+        <v>6.2947455965311594E-2</v>
+      </c>
+      <c r="AR22" s="6">
+        <v>6.4769820076350695E-2</v>
+      </c>
+      <c r="AS22" s="6">
+        <v>6.1096818099759899E-2</v>
+      </c>
+      <c r="AT22" s="6">
+        <v>6.1095932437070899E-2</v>
+      </c>
+      <c r="AU22" s="6">
+        <v>6.3867056963875596E-2</v>
+      </c>
+      <c r="AV22" s="6">
+        <v>6.4741362019758497E-2</v>
+      </c>
+      <c r="AW22" s="6">
+        <v>6.7018838716514595E-2</v>
+      </c>
+      <c r="AX22" s="6">
+        <v>6.6962982006557398E-2</v>
+      </c>
+      <c r="AY22" s="6">
+        <v>6.5536466378873198E-2</v>
+      </c>
+      <c r="AZ22" s="6">
+        <v>6.4700936678537893E-2</v>
+      </c>
+      <c r="BA22" s="6">
+        <v>6.6352562351897099E-2</v>
+      </c>
+      <c r="BB22" s="6">
+        <v>6.7167976366605597E-2</v>
+      </c>
+      <c r="BC22" s="6">
+        <v>6.7491421514417296E-2</v>
+      </c>
+      <c r="BD22" s="6">
+        <v>6.8141597655203598E-2</v>
+      </c>
+      <c r="BE22" s="6">
+        <v>6.6034662506168199E-2</v>
+      </c>
+      <c r="BF22" s="6">
+        <v>6.3584032035466601E-2</v>
+      </c>
+      <c r="BG22" s="6">
+        <v>6.2352985977295002E-2</v>
+      </c>
+      <c r="BH22" s="6">
+        <v>6.1066635075669402E-2</v>
+      </c>
+      <c r="BI22" s="6">
+        <v>6.1153788434545497E-2</v>
+      </c>
+      <c r="BJ22" s="6">
+        <v>6.0794657801175003E-2</v>
+      </c>
+      <c r="BK22" s="6">
+        <v>6.1664330268599299E-2</v>
+      </c>
+      <c r="BL22" s="6">
+        <v>6.3304066311039603E-2</v>
+      </c>
+      <c r="BM22" s="6">
+        <v>6.19659319090499E-2</v>
+      </c>
+      <c r="BN22" s="6">
+        <v>6.2526699282010503E-2</v>
+      </c>
+      <c r="BO22" s="6">
+        <v>6.1346509429632899E-2</v>
+      </c>
+      <c r="BP22" s="6">
+        <v>6.0521781579537602E-2</v>
+      </c>
+      <c r="BQ22" s="6">
+        <v>6.0529178194759801E-2</v>
+      </c>
+      <c r="BR22" s="6">
+        <v>5.9016064553069701E-2</v>
+      </c>
+      <c r="BS22" s="6">
+        <v>5.8525012643658697E-2</v>
+      </c>
+      <c r="BT22" s="6">
+        <v>5.8311550680135597E-2</v>
+      </c>
+      <c r="BU22" s="6">
+        <v>5.7156984354240999E-2</v>
+      </c>
+      <c r="BV22" s="6">
+        <v>5.6850597759923703E-2</v>
+      </c>
+      <c r="BW22" s="6">
+        <v>5.73458855420425E-2</v>
+      </c>
+      <c r="BX22" s="6">
+        <v>5.6655385655410201E-2</v>
+      </c>
+      <c r="BY22" s="6">
+        <v>5.5248557360571403E-2</v>
+      </c>
+      <c r="BZ22" s="6">
+        <v>5.3374433142524401E-2</v>
+      </c>
+      <c r="CA22" s="6">
+        <v>5.1927661429221603E-2</v>
+      </c>
+      <c r="CB22" s="6">
+        <v>5.1288316014665498E-2</v>
+      </c>
+      <c r="CC22" s="6">
+        <v>5.04985954324738E-2</v>
+      </c>
+      <c r="CD22" s="6">
+        <v>4.9359476778931398E-2</v>
+      </c>
+      <c r="CE22" s="6">
+        <v>4.9301326002151799E-2</v>
+      </c>
+      <c r="CF22" s="6">
+        <v>4.8891577122884999E-2</v>
+      </c>
+      <c r="CG22" s="6">
+        <v>4.8263573143916397E-2</v>
+      </c>
+      <c r="CH22" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="CI22" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5.6854385964912303E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>6.50425076452599E-2</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6.50425076452599E-2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>6.6812951167728202E-2</v>
+      </c>
+      <c r="H23" s="3">
+        <v>7.5457333333333307E-2</v>
+      </c>
+      <c r="I23" s="3">
+        <v>7.1786390532544403E-2</v>
+      </c>
+      <c r="J23" s="3">
+        <v>6.94541052631579E-2</v>
+      </c>
+      <c r="K23" s="3">
+        <v>6.9207692307692303E-2</v>
+      </c>
+      <c r="L23" s="3">
+        <v>6.2522335025380696E-2</v>
+      </c>
+      <c r="M23" s="3">
+        <v>5.7424518388791597E-2</v>
+      </c>
+      <c r="N23" s="3">
+        <v>5.5443548387096801E-2</v>
+      </c>
+      <c r="O23" s="3">
+        <v>5.4127059590986397E-2</v>
+      </c>
+      <c r="P23" s="3">
+        <v>5.53221516126454E-2</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>5.7439531576759101E-2</v>
+      </c>
+      <c r="R23" s="3">
+        <v>5.76514763823677E-2</v>
+      </c>
+      <c r="S23" s="3">
+        <v>5.5013291260700398E-2</v>
+      </c>
+      <c r="T23" s="3">
+        <v>5.3994768370607002E-2</v>
+      </c>
+      <c r="U23" s="3">
+        <v>5.2362193926701599E-2</v>
+      </c>
+      <c r="V23" s="3">
+        <v>4.8054450636442897E-2</v>
+      </c>
+      <c r="W23" s="3">
+        <v>5.3855949997012299E-2</v>
+      </c>
+      <c r="X23" s="6">
+        <v>5.2971130226895403E-2</v>
+      </c>
+      <c r="Y23" s="6">
+        <v>5.1167328759782901E-2</v>
+      </c>
+      <c r="Z23" s="6">
+        <v>5.3102469166666701E-2</v>
+      </c>
+      <c r="AA23" s="6">
+        <v>4.4570205511103501E-2</v>
+      </c>
+      <c r="AB23" s="6">
+        <v>4.7204346213570302E-2</v>
+      </c>
+      <c r="AC23" s="6">
+        <v>5.2498275535763902E-2</v>
+      </c>
+      <c r="AD23" s="6">
+        <v>5.8880532243412401E-2</v>
+      </c>
+      <c r="AE23" s="6">
+        <v>6.6424314459522696E-2</v>
+      </c>
+      <c r="AF23" s="6">
+        <v>5.84942226255293E-2</v>
+      </c>
+      <c r="AG23" s="6">
+        <v>5.7403852201257898E-2</v>
+      </c>
+      <c r="AH23" s="6">
+        <v>5.3577872465471597E-2</v>
+      </c>
+      <c r="AI23" s="6">
+        <v>5.3837408820143901E-2</v>
+      </c>
+      <c r="AJ23" s="6">
+        <v>5.6939794253169897E-2</v>
+      </c>
+      <c r="AK23" s="6">
+        <v>5.7794129797570801E-2</v>
+      </c>
+      <c r="AL23" s="6">
+        <v>5.9330217243139798E-2</v>
+      </c>
+      <c r="AM23" s="6">
+        <v>5.9869346731250002E-2</v>
+      </c>
+      <c r="AN23" s="6">
+        <v>6.3848176830426706E-2</v>
+      </c>
+      <c r="AO23" s="6">
+        <v>5.9555010758885203E-2</v>
+      </c>
+      <c r="AP23" s="6">
+        <v>5.8790463293027603E-2</v>
+      </c>
+      <c r="AQ23" s="6">
+        <v>5.7904062133777801E-2</v>
+      </c>
+      <c r="AR23" s="6">
+        <v>5.4544484157205197E-2</v>
+      </c>
+      <c r="AS23" s="6">
+        <v>5.4434281339201397E-2</v>
+      </c>
+      <c r="AT23" s="6">
+        <v>5.1665960205865398E-2</v>
+      </c>
+      <c r="AU23" s="6">
+        <v>5.05582696538288E-2</v>
+      </c>
+      <c r="AV23" s="6">
+        <v>5.1528423240064902E-2</v>
+      </c>
+      <c r="AW23" s="6">
+        <v>4.98289816141659E-2</v>
+      </c>
+      <c r="AX23" s="6">
+        <v>4.9262966780133401E-2</v>
+      </c>
+      <c r="AY23" s="6">
+        <v>4.9653391633868199E-2</v>
+      </c>
+      <c r="AZ23" s="6">
+        <v>4.6656566052652997E-2</v>
+      </c>
+      <c r="BA23" s="6">
+        <v>4.6434565796666702E-2</v>
+      </c>
+      <c r="BB23" s="6">
+        <v>4.4460433993496397E-2</v>
+      </c>
+      <c r="BC23" s="6">
+        <v>4.3656201521396099E-2</v>
+      </c>
+      <c r="BD23" s="6">
+        <v>4.7215393600151402E-2</v>
+      </c>
+      <c r="BE23" s="6">
+        <v>4.7341396091965603E-2</v>
+      </c>
+      <c r="BF23" s="6">
+        <v>4.7139146176411698E-2</v>
+      </c>
+      <c r="BG23" s="6">
+        <v>4.7197219285132402E-2</v>
+      </c>
+      <c r="BH23" s="6">
+        <v>4.7049149094333997E-2</v>
+      </c>
+      <c r="BI23" s="6">
+        <v>4.7696228778707099E-2</v>
+      </c>
+      <c r="BJ23" s="6">
+        <v>4.8117349204775901E-2</v>
+      </c>
+      <c r="BK23" s="6">
+        <v>4.7686856303043298E-2</v>
+      </c>
+      <c r="BL23" s="6">
+        <v>4.6143235060160701E-2</v>
+      </c>
+      <c r="BM23" s="6">
+        <v>4.5093246094034603E-2</v>
+      </c>
+      <c r="BN23" s="6">
+        <v>4.4645816293115502E-2</v>
+      </c>
+      <c r="BO23" s="6">
+        <v>4.4473308294829199E-2</v>
+      </c>
+      <c r="BP23" s="6">
+        <v>4.5964551252969298E-2</v>
+      </c>
+      <c r="BQ23" s="6">
+        <v>4.5758619773926701E-2</v>
+      </c>
+      <c r="BR23" s="6">
+        <v>4.5479114535580498E-2</v>
+      </c>
+      <c r="BS23" s="6">
+        <v>4.5591481631710798E-2</v>
+      </c>
+      <c r="BT23" s="6">
+        <v>4.4734645826483503E-2</v>
+      </c>
+      <c r="BU23" s="6">
+        <v>4.5151072564442701E-2</v>
+      </c>
+      <c r="BV23" s="6">
+        <v>4.5184528986263003E-2</v>
+      </c>
+      <c r="BW23" s="6">
+        <v>4.5291354311035197E-2</v>
+      </c>
+      <c r="BX23" s="6">
+        <v>4.4943891297600402E-2</v>
+      </c>
+      <c r="BY23" s="6">
+        <v>4.3846672767509698E-2</v>
+      </c>
+      <c r="BZ23" s="6">
+        <v>4.4586301607536197E-2</v>
+      </c>
+      <c r="CA23" s="6">
+        <v>4.4462155046821501E-2</v>
+      </c>
+      <c r="CB23" s="6">
+        <v>4.45949091702331E-2</v>
+      </c>
+      <c r="CC23" s="6">
+        <v>4.5188393764118602E-2</v>
+      </c>
+      <c r="CD23" s="6">
+        <v>4.469111135922E-2</v>
+      </c>
+      <c r="CE23" s="6">
+        <v>4.4798348488586999E-2</v>
+      </c>
+      <c r="CF23" s="6">
+        <v>4.5027156375293802E-2</v>
+      </c>
+      <c r="CG23" s="6">
+        <v>4.43870562400124E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="3">
+        <v>8.3099999999999993E-2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>8.7077175141242899E-2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8.7758349999999999E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>8.7758349999999999E-2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>8.8580411764705894E-2</v>
+      </c>
+      <c r="H24" s="3">
+        <v>8.7330876132930502E-2</v>
+      </c>
+      <c r="I24" s="3">
+        <v>8.1924305555555604E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <v>8.39669076305221E-2</v>
+      </c>
+      <c r="K24" s="3">
+        <v>8.6653665689149603E-2</v>
+      </c>
+      <c r="L24" s="3">
+        <v>8.5595437956204404E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>8.46875199634953E-2</v>
+      </c>
+      <c r="N24" s="3">
+        <v>8.2799553256524799E-2</v>
+      </c>
+      <c r="O24" s="3">
+        <v>7.8201951703605693E-2</v>
+      </c>
+      <c r="P24" s="3">
+        <v>7.7196945010183302E-2</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>7.61043912780133E-2</v>
+      </c>
+      <c r="R24" s="3">
+        <v>7.4324164278892102E-2</v>
+      </c>
+      <c r="S24" s="3">
+        <v>7.6962571196094398E-2</v>
+      </c>
+      <c r="T24" s="3">
+        <v>7.8003237518910695E-2</v>
+      </c>
+      <c r="U24" s="3">
+        <v>8.0583448012232398E-2</v>
+      </c>
+      <c r="V24" s="3">
+        <v>7.45529900198377E-2</v>
+      </c>
+      <c r="W24" s="3">
+        <v>7.10522084211338E-2</v>
+      </c>
+      <c r="X24" s="6">
+        <v>6.8492871132062497E-2</v>
+      </c>
+      <c r="Y24" s="6">
+        <v>6.8470051198161394E-2</v>
+      </c>
+      <c r="Z24" s="6">
+        <v>6.9445737854813699E-2</v>
+      </c>
+      <c r="AA24" s="6">
+        <v>6.8204170554560004E-2</v>
+      </c>
+      <c r="AB24" s="6">
+        <v>7.11413465441849E-2</v>
+      </c>
+      <c r="AC24" s="6">
+        <v>6.8023998642236905E-2</v>
+      </c>
+      <c r="AD24" s="6">
+        <v>6.8942276228243296E-2</v>
+      </c>
+      <c r="AE24" s="6">
+        <v>7.1319585915162895E-2</v>
+      </c>
+      <c r="AF24" s="6">
+        <v>6.4058529824670293E-2</v>
+      </c>
+      <c r="AG24" s="6">
+        <v>7.6428692146214103E-2</v>
+      </c>
+      <c r="AH24" s="6">
+        <v>7.2053225806451598E-2</v>
+      </c>
+      <c r="AI24" s="6">
+        <v>7.3431122031121995E-2</v>
+      </c>
+      <c r="AJ24" s="6">
+        <v>8.09154826958106E-2</v>
+      </c>
+      <c r="AK24" s="6">
+        <v>7.6848807339449501E-2</v>
+      </c>
+      <c r="AL24" s="6">
+        <v>7.4000129808510604E-2</v>
+      </c>
+      <c r="AM24" s="6">
+        <v>7.2446930493046804E-2</v>
+      </c>
+      <c r="AN24" s="6">
+        <v>7.6087697414829694E-2</v>
+      </c>
+      <c r="AO24" s="6">
+        <v>7.56648070020534E-2</v>
+      </c>
+      <c r="AP24" s="6">
+        <v>7.7826064691232502E-2</v>
+      </c>
+      <c r="AQ24" s="6">
+        <v>7.3242586474159099E-2</v>
+      </c>
+      <c r="AR24" s="6">
+        <v>7.3927268560520606E-2</v>
+      </c>
+      <c r="AS24" s="6">
+        <v>7.4573558103328594E-2</v>
+      </c>
+      <c r="AT24" s="6">
+        <v>7.3628497913185903E-2</v>
+      </c>
+      <c r="AU24" s="6">
+        <v>7.2946238406120495E-2</v>
+      </c>
+      <c r="AV24" s="6">
+        <v>7.2426440230731595E-2</v>
+      </c>
+      <c r="AW24" s="6">
+        <v>7.1840636044308098E-2</v>
+      </c>
+      <c r="AX24" s="6">
+        <v>7.2795069941236301E-2</v>
+      </c>
+      <c r="AY24" s="6">
+        <v>7.5428132436375597E-2</v>
+      </c>
+      <c r="AZ24" s="6">
+        <v>7.6722858733964297E-2</v>
+      </c>
+      <c r="BA24" s="6">
+        <v>7.2983377926299803E-2</v>
+      </c>
+      <c r="BB24" s="6">
+        <v>7.1912025464897805E-2</v>
+      </c>
+      <c r="BC24" s="6">
+        <v>6.6543629166025201E-2</v>
+      </c>
+      <c r="BD24" s="6">
+        <v>6.5362041744657803E-2</v>
+      </c>
+      <c r="BE24" s="6">
+        <v>6.7073640566324894E-2</v>
+      </c>
+      <c r="BF24" s="6">
+        <v>6.6788250035595007E-2</v>
+      </c>
+      <c r="BG24" s="6">
+        <v>6.8080134412051505E-2</v>
+      </c>
+      <c r="BH24" s="6">
+        <v>6.7207053111214304E-2</v>
+      </c>
+      <c r="BI24" s="6">
+        <v>6.6937760502041602E-2</v>
+      </c>
+      <c r="BJ24" s="6">
+        <v>6.6571571594372894E-2</v>
+      </c>
+      <c r="BK24" s="6">
+        <v>6.6816925696959004E-2</v>
+      </c>
+      <c r="BL24" s="6">
+        <v>6.5694487198262805E-2</v>
+      </c>
+      <c r="BM24" s="6">
+        <v>6.5545338116859905E-2</v>
+      </c>
+      <c r="BN24" s="6">
+        <v>6.3202652172533999E-2</v>
+      </c>
+      <c r="BO24" s="6">
+        <v>6.3095920287724302E-2</v>
+      </c>
+      <c r="BP24" s="6">
+        <v>6.3021446407492507E-2</v>
+      </c>
+      <c r="BQ24" s="6">
+        <v>6.1061597664194799E-2</v>
+      </c>
+      <c r="BR24" s="6">
+        <v>6.1144422290315102E-2</v>
+      </c>
+      <c r="BS24" s="6">
+        <v>6.0375068966207798E-2</v>
+      </c>
+      <c r="BT24" s="6">
+        <v>5.9796106863504103E-2</v>
+      </c>
+      <c r="BU24" s="6">
+        <v>6.0063973237081701E-2</v>
+      </c>
+      <c r="BV24" s="6">
+        <v>6.0091690082659098E-2</v>
+      </c>
+      <c r="BW24" s="6">
+        <v>6.0630497609376298E-2</v>
+      </c>
+      <c r="BX24" s="6">
+        <v>6.1429678970772401E-2</v>
+      </c>
+      <c r="BY24" s="6">
+        <v>5.9368725305466802E-2</v>
+      </c>
+      <c r="BZ24" s="6">
+        <v>5.8936275711225103E-2</v>
+      </c>
+      <c r="CA24" s="6">
+        <v>5.8328600125501603E-2</v>
+      </c>
+      <c r="CB24" s="6">
+        <v>5.7402315263402198E-2</v>
+      </c>
+      <c r="CC24" s="6">
+        <v>5.6886411771328999E-2</v>
+      </c>
+      <c r="CD24" s="6">
+        <v>5.4995826859333602E-2</v>
+      </c>
+      <c r="CE24" s="6">
+        <v>5.45247852337487E-2</v>
+      </c>
+      <c r="CF24" s="6">
+        <v>5.3771741776680697E-2</v>
+      </c>
+      <c r="CG24" s="6">
+        <v>5.3973445786977298E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.102222813688213</v>
+      </c>
+      <c r="D25" s="3">
+        <v>9.1719999999999996E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>9.1719999999999996E-2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>9.0653485064011399E-2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>8.3738181818181795E-2</v>
+      </c>
+      <c r="H25" s="3">
+        <v>8.38992248062016E-2</v>
+      </c>
+      <c r="I25" s="3">
+        <v>8.55710638297872E-2</v>
+      </c>
+      <c r="J25" s="3">
+        <v>8.2381564245810099E-2</v>
+      </c>
+      <c r="K25" s="3">
+        <v>8.4242392188771303E-2</v>
+      </c>
+      <c r="L25" s="3">
+        <v>8.1531448538754797E-2</v>
+      </c>
+      <c r="M25" s="3">
+        <v>8.0239334955393399E-2</v>
+      </c>
+      <c r="N25" s="3">
+        <v>7.7272184531886001E-2</v>
+      </c>
+      <c r="O25" s="3">
+        <v>6.4632550335570499E-2</v>
+      </c>
+      <c r="P25" s="3">
+        <v>5.80383858267716E-2</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>6.3785162180814398E-2</v>
+      </c>
+      <c r="R25" s="3">
+        <v>6.8221734911058901E-2</v>
+      </c>
+      <c r="S25" s="3">
+        <v>7.0957802261308003E-2</v>
+      </c>
+      <c r="T25" s="3">
+        <v>7.2005841237431895E-2</v>
+      </c>
+      <c r="U25" s="3">
+        <v>7.3538336229932597E-2</v>
+      </c>
+      <c r="V25" s="3">
+        <v>7.4345171339563906E-2</v>
+      </c>
+      <c r="W25" s="3">
+        <v>7.5174280710532906E-2</v>
+      </c>
+      <c r="X25" s="6">
+        <v>7.6885774183887395E-2</v>
+      </c>
+      <c r="Y25" s="6">
+        <v>7.2883641029839699E-2</v>
+      </c>
+      <c r="Z25" s="6">
+        <v>6.8236239025670303E-2</v>
+      </c>
+      <c r="AA25" s="6">
+        <v>6.7116122412759396E-2</v>
+      </c>
+      <c r="AB25" s="6">
+        <v>6.2636805787721295E-2</v>
+      </c>
+      <c r="AC25" s="6">
+        <v>6.4003641106180301E-2</v>
+      </c>
+      <c r="AD25" s="6">
+        <v>6.4712744547169798E-2</v>
+      </c>
+      <c r="AE25" s="6">
+        <v>6.6492799002658698E-2</v>
+      </c>
+      <c r="AF25" s="6">
+        <v>7.7457857142857106E-2</v>
+      </c>
+      <c r="AG25" s="6">
+        <v>7.9648654970760194E-2</v>
+      </c>
+      <c r="AH25" s="6">
+        <v>7.7188184187662906E-2</v>
+      </c>
+      <c r="AI25" s="6">
+        <v>7.44532010820559E-2</v>
+      </c>
+      <c r="AJ25" s="6">
+        <v>7.4901122442748103E-2</v>
+      </c>
+      <c r="AK25" s="6">
+        <v>7.6630994835886201E-2</v>
+      </c>
+      <c r="AL25" s="6">
+        <v>8.2465684793608496E-2</v>
+      </c>
+      <c r="AM25" s="6">
+        <v>6.2953551649365599E-2</v>
+      </c>
+      <c r="AN25" s="6">
+        <v>6.1002766251728902E-2</v>
+      </c>
+      <c r="AO25" s="6">
+        <v>4.7219570405727898E-2</v>
+      </c>
+      <c r="AP25" s="6">
+        <v>6.3920737488569607E-2</v>
+      </c>
+      <c r="AQ25" s="6">
+        <v>7.2440885473017996E-2</v>
+      </c>
+      <c r="AR25" s="6">
+        <v>7.36230731492971E-2</v>
+      </c>
+      <c r="AS25" s="6">
+        <v>7.3636698514700699E-2</v>
+      </c>
+      <c r="AT25" s="6">
+        <v>7.3502704383537606E-2</v>
+      </c>
+      <c r="AU25" s="6">
+        <v>7.3627884557566206E-2</v>
+      </c>
+      <c r="AV25" s="6">
+        <v>7.2781074075851895E-2</v>
+      </c>
+      <c r="AW25" s="6">
+        <v>7.1009619783572397E-2</v>
+      </c>
+      <c r="AX25" s="6">
+        <v>6.7551428230886501E-2</v>
+      </c>
+      <c r="AY25" s="6">
+        <v>6.3200091872422703E-2</v>
+      </c>
+      <c r="AZ25" s="6">
+        <v>6.2991493329224907E-2</v>
+      </c>
+      <c r="BA25" s="6">
+        <v>6.3497499103861904E-2</v>
+      </c>
+      <c r="BB25" s="6">
+        <v>6.6029072246631404E-2</v>
+      </c>
+      <c r="BC25" s="6">
+        <v>6.7559222664729093E-2</v>
+      </c>
+      <c r="BD25" s="6">
+        <v>6.9640265414031094E-2</v>
+      </c>
+      <c r="BE25" s="6">
+        <v>6.7129047988270699E-2</v>
+      </c>
+      <c r="BF25" s="6">
+        <v>6.6804533796253604E-2</v>
+      </c>
+      <c r="BG25" s="6">
+        <v>6.6629964265903993E-2</v>
+      </c>
+      <c r="BH25" s="6">
+        <v>6.4871823522138605E-2</v>
+      </c>
+      <c r="BI25" s="6">
+        <v>6.51196183004078E-2</v>
+      </c>
+      <c r="BJ25" s="6">
+        <v>6.5004977640269801E-2</v>
+      </c>
+      <c r="BK25" s="6">
+        <v>6.3600554934571202E-2</v>
+      </c>
+      <c r="BL25" s="6">
+        <v>6.3548996717382497E-2</v>
+      </c>
+      <c r="BM25" s="6">
+        <v>6.1829212250308303E-2</v>
+      </c>
+      <c r="BN25" s="6">
+        <v>6.1242336962544698E-2</v>
+      </c>
+      <c r="BO25" s="6">
+        <v>6.0864109954749002E-2</v>
+      </c>
+      <c r="BP25" s="6">
+        <v>6.0133302878122602E-2</v>
+      </c>
+      <c r="BQ25" s="6">
+        <v>6.1436275507965099E-2</v>
+      </c>
+      <c r="BR25" s="6">
+        <v>6.0905658308540597E-2</v>
+      </c>
+      <c r="BS25" s="6">
+        <v>6.1289530445977201E-2</v>
+      </c>
+      <c r="BT25" s="6">
+        <v>6.0922320842530797E-2</v>
+      </c>
+      <c r="BU25" s="6">
+        <v>6.0565872049843698E-2</v>
+      </c>
+      <c r="BV25" s="6">
+        <v>6.1115354009695103E-2</v>
+      </c>
+      <c r="BW25" s="6">
+        <v>6.0434249178047898E-2</v>
+      </c>
+      <c r="BX25" s="6">
+        <v>6.0821933198485799E-2</v>
+      </c>
+      <c r="BY25" s="6">
+        <v>5.8897221484915697E-2</v>
+      </c>
+      <c r="BZ25" s="6">
+        <v>5.72920897826701E-2</v>
+      </c>
+      <c r="CA25" s="6">
+        <v>5.69255775881242E-2</v>
+      </c>
+      <c r="CB25" s="6">
+        <v>5.49826703822687E-2</v>
+      </c>
+      <c r="CC25" s="6">
+        <v>5.4094069120939101E-2</v>
+      </c>
+      <c r="CD25" s="6">
+        <v>5.3536067777418699E-2</v>
+      </c>
+      <c r="CE25" s="6">
+        <v>5.2443985365748201E-2</v>
+      </c>
+      <c r="CF25" s="6">
+        <v>5.2813867158925901E-2</v>
+      </c>
+      <c r="CG25" s="6">
+        <v>5.2430127881694398E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
building an individual MSA component
also revising data to include only MSAs for which the BLS publishes a CPI currently
</commit_message>
<xml_diff>
--- a/data/realpage_market_cr.xlsx
+++ b/data/realpage_market_cr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\inflation_cr_expansion\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlarriva\Documents\GitHub\inflation_cr_expansion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FD7338-6546-4A44-9351-AA00243280E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012EF860-820B-4C29-8F8F-A80D237A02CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32175" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-9630" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEOGRAPHIES" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="136">
   <si>
     <t>Geography Name</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>SanJose</t>
+  </si>
+  <si>
+    <t>Detroit-Warren-Dearborn, MI</t>
+  </si>
+  <si>
+    <t>Detroit</t>
   </si>
 </sst>
 </file>
@@ -824,16 +830,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CI25"/>
+  <dimension ref="A1:CI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="23" width="16" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1090,7 +1098,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1347,7 +1355,7 @@
         <v>4.7870708050830602E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1604,7 +1612,7 @@
         <v>5.14074607471968E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1861,7 +1869,7 @@
         <v>4.4068083643351998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2118,7 +2126,7 @@
         <v>5.0581629697618702E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2375,7 +2383,7 @@
         <v>4.6145597661125103E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2632,7 +2640,7 @@
         <v>4.35329961887874E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2889,7 +2897,7 @@
         <v>4.92741828603213E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -3146,7 +3154,7 @@
         <v>4.3067592293483198E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -3403,7 +3411,7 @@
         <v>4.6944635306451599E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -3660,7 +3668,7 @@
         <v>4.7550908072163903E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -3917,7 +3925,7 @@
         <v>4.6755518098505998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -4174,7 +4182,7 @@
         <v>4.9790917210938701E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4431,7 +4439,7 @@
         <v>4.3513993359494199E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4688,7 +4696,7 @@
         <v>4.2619840349245298E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -4945,7 +4953,7 @@
         <v>3.9655819377456103E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -5202,7 +5210,7 @@
         <v>4.1980557011838497E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -5459,7 +5467,7 @@
         <v>5.3355687826240103E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -5716,7 +5724,7 @@
         <v>4.7860483840902399E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -5973,7 +5981,7 @@
         <v>4.6838490123922903E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -6230,7 +6238,7 @@
         <v>4.8100262187196902E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -6493,7 +6501,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -6750,7 +6758,7 @@
         <v>4.43870562400124E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -7007,7 +7015,7 @@
         <v>5.3973445786977298E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:87" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -7262,6 +7270,267 @@
       </c>
       <c r="CG25" s="6">
         <v>5.2430127881694398E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="3">
+        <v>8.6891904761904795E-2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>8.6371129707112998E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8.6690476190476207E-2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8.5960947259565698E-2</v>
+      </c>
+      <c r="G26" s="3">
+        <v>8.5721197593706597E-2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>8.5898243520782402E-2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>8.3731374382022494E-2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>8.1858987662015506E-2</v>
+      </c>
+      <c r="K26" s="3">
+        <v>7.9192903162629794E-2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>8.2126537588185694E-2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>8.1587570275976698E-2</v>
+      </c>
+      <c r="N26" s="3">
+        <v>8.1097931034482804E-2</v>
+      </c>
+      <c r="O26" s="3">
+        <v>8.2752000000000006E-2</v>
+      </c>
+      <c r="P26" s="3">
+        <v>7.5851884751772999E-2</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>7.55788494319663E-2</v>
+      </c>
+      <c r="R26" s="3">
+        <v>7.3813330662476404E-2</v>
+      </c>
+      <c r="S26" s="3">
+        <v>7.2618262944524906E-2</v>
+      </c>
+      <c r="T26" s="3">
+        <v>7.1114571914322605E-2</v>
+      </c>
+      <c r="U26" s="3">
+        <v>6.3463380923450802E-2</v>
+      </c>
+      <c r="V26" s="3">
+        <v>6.4546459226739294E-2</v>
+      </c>
+      <c r="W26" s="3">
+        <v>6.4111119958863302E-2</v>
+      </c>
+      <c r="X26" s="6">
+        <v>6.6044938344163098E-2</v>
+      </c>
+      <c r="Y26" s="6">
+        <v>7.1835993481562693E-2</v>
+      </c>
+      <c r="Z26" s="6">
+        <v>7.3208113375948E-2</v>
+      </c>
+      <c r="AA26" s="6">
+        <v>7.16589857753792E-2</v>
+      </c>
+      <c r="AB26" s="6">
+        <v>7.04586162836119E-2</v>
+      </c>
+      <c r="AC26" s="6">
+        <v>6.9022702702119104E-2</v>
+      </c>
+      <c r="AD26" s="6">
+        <v>6.9839038081795396E-2</v>
+      </c>
+      <c r="AE26" s="6">
+        <v>7.0523367109019394E-2</v>
+      </c>
+      <c r="AF26" s="6">
+        <v>8.2441144239219402E-2</v>
+      </c>
+      <c r="AG26" s="6">
+        <v>8.8201009824501894E-2</v>
+      </c>
+      <c r="AH26" s="6">
+        <v>8.7507053072625698E-2</v>
+      </c>
+      <c r="AI26" s="6">
+        <v>9.3173649289099505E-2</v>
+      </c>
+      <c r="AJ26" s="6">
+        <v>8.3526306620209101E-2</v>
+      </c>
+      <c r="AK26" s="6">
+        <v>8.4341598360655703E-2</v>
+      </c>
+      <c r="AL26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO26" s="6">
+        <v>9.7564737031700294E-2</v>
+      </c>
+      <c r="AP26" s="6">
+        <v>9.67728858768407E-2</v>
+      </c>
+      <c r="AQ26" s="6">
+        <v>9.4790932657926097E-2</v>
+      </c>
+      <c r="AR26" s="6">
+        <v>9.3302271321614602E-2</v>
+      </c>
+      <c r="AS26" s="6">
+        <v>8.7079580796296296E-2</v>
+      </c>
+      <c r="AT26" s="6">
+        <v>7.8796806427469099E-2</v>
+      </c>
+      <c r="AU26" s="6">
+        <v>7.9067534542961102E-2</v>
+      </c>
+      <c r="AV26" s="6">
+        <v>8.0851605434038396E-2</v>
+      </c>
+      <c r="AW26" s="6">
+        <v>8.0098265332576093E-2</v>
+      </c>
+      <c r="AX26" s="6">
+        <v>8.0677228562061207E-2</v>
+      </c>
+      <c r="AY26" s="6">
+        <v>7.6309386043858701E-2</v>
+      </c>
+      <c r="AZ26" s="6">
+        <v>7.4428639481987399E-2</v>
+      </c>
+      <c r="BA26" s="6">
+        <v>7.4964094324016795E-2</v>
+      </c>
+      <c r="BB26" s="6">
+        <v>7.6374748748685606E-2</v>
+      </c>
+      <c r="BC26" s="6">
+        <v>7.8222792133929506E-2</v>
+      </c>
+      <c r="BD26" s="6">
+        <v>7.8412909051586197E-2</v>
+      </c>
+      <c r="BE26" s="6">
+        <v>7.7991645803927298E-2</v>
+      </c>
+      <c r="BF26" s="6">
+        <v>7.6313219436533297E-2</v>
+      </c>
+      <c r="BG26" s="6">
+        <v>7.5694098656561501E-2</v>
+      </c>
+      <c r="BH26" s="6">
+        <v>7.1021712280196506E-2</v>
+      </c>
+      <c r="BI26" s="6">
+        <v>7.0740044890639495E-2</v>
+      </c>
+      <c r="BJ26" s="6">
+        <v>6.9253260109880296E-2</v>
+      </c>
+      <c r="BK26" s="6">
+        <v>6.99945580345714E-2</v>
+      </c>
+      <c r="BL26" s="6">
+        <v>7.1317152145560794E-2</v>
+      </c>
+      <c r="BM26" s="6">
+        <v>7.0721272084129996E-2</v>
+      </c>
+      <c r="BN26" s="6">
+        <v>6.9993685425742594E-2</v>
+      </c>
+      <c r="BO26" s="6">
+        <v>6.7966677749999996E-2</v>
+      </c>
+      <c r="BP26" s="6">
+        <v>6.7112034695529801E-2</v>
+      </c>
+      <c r="BQ26" s="6">
+        <v>6.62331317652462E-2</v>
+      </c>
+      <c r="BR26" s="6">
+        <v>6.5757119355109597E-2</v>
+      </c>
+      <c r="BS26" s="6">
+        <v>6.6101983576761197E-2</v>
+      </c>
+      <c r="BT26" s="6">
+        <v>6.4935880315140707E-2</v>
+      </c>
+      <c r="BU26" s="6">
+        <v>6.4642532874853706E-2</v>
+      </c>
+      <c r="BV26" s="6">
+        <v>6.2988313062208201E-2</v>
+      </c>
+      <c r="BW26" s="6">
+        <v>6.3302016067390804E-2</v>
+      </c>
+      <c r="BX26" s="6">
+        <v>6.1417481676923097E-2</v>
+      </c>
+      <c r="BY26" s="6">
+        <v>6.1157200167224299E-2</v>
+      </c>
+      <c r="BZ26" s="6">
+        <v>6.0647290356573999E-2</v>
+      </c>
+      <c r="CA26" s="6">
+        <v>5.9340264784722201E-2</v>
+      </c>
+      <c r="CB26" s="6">
+        <v>5.9711754204394701E-2</v>
+      </c>
+      <c r="CC26" s="6">
+        <v>5.7166004197399103E-2</v>
+      </c>
+      <c r="CD26" s="6">
+        <v>5.6232553773217897E-2</v>
+      </c>
+      <c r="CE26" s="6">
+        <v>5.4767993074784298E-2</v>
+      </c>
+      <c r="CF26" s="6">
+        <v>5.4040305682230498E-2</v>
+      </c>
+      <c r="CG26" s="6">
+        <v>5.4783708443934501E-2</v>
+      </c>
+      <c r="CH26" s="6"/>
+      <c r="CI26" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating data testing periodization
moving the GDP figures back on year because they come out so late
</commit_message>
<xml_diff>
--- a/data/realpage_market_cr.xlsx
+++ b/data/realpage_market_cr.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlarriva\Documents\GitHub\inflation_cr_expansion\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\inflation_cr_expansion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012EF860-820B-4C29-8F8F-A80D237A02CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF6CBA-928F-4BFF-82EF-A490AE412A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-9630" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEOGRAPHIES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GEOGRAPHIES!$B$1:$AB$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GEOGRAPHIES!$A$1:$CI$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="136">
   <si>
     <t>Geography Name</t>
   </si>
@@ -830,18 +830,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:CI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AL26" sqref="AL26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="23" width="16" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -1098,7 +1099,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>4.7870708050830602E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>5.14074607471968E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1869,7 +1870,7 @@
         <v>4.4068083643351998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>5.0581629697618702E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2383,7 +2384,7 @@
         <v>4.6145597661125103E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>4.35329961887874E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>4.92741828603213E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>4.3067592293483198E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -3411,7 +3412,7 @@
         <v>4.6944635306451599E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>4.7550908072163903E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -3925,7 +3926,7 @@
         <v>4.6755518098505998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -4182,7 +4183,7 @@
         <v>4.9790917210938701E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4439,7 +4440,7 @@
         <v>4.3513993359494199E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4696,7 +4697,7 @@
         <v>4.2619840349245298E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:85" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>3.9655819377456103E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -5210,7 +5211,7 @@
         <v>4.1980557011838497E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -5467,7 +5468,7 @@
         <v>5.3355687826240103E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -5724,7 +5725,7 @@
         <v>4.7860483840902399E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -5981,7 +5982,7 @@
         <v>4.6838490123922903E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -6238,7 +6239,7 @@
         <v>4.8100262187196902E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -6501,7 +6502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -6758,7 +6759,7 @@
         <v>4.43870562400124E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -7015,7 +7016,7 @@
         <v>5.3973445786977298E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:87" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -7272,7 +7273,7 @@
         <v>5.2430127881694398E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -7384,8 +7385,9 @@
       <c r="AK26" s="6">
         <v>8.4341598360655703E-2</v>
       </c>
-      <c r="AL26" s="6" t="s">
-        <v>23</v>
+      <c r="AL26" s="6">
+        <f>AK26</f>
+        <v>8.4341598360655703E-2</v>
       </c>
       <c r="AM26" s="6" t="s">
         <v>23</v>
@@ -7534,10 +7536,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AB20" xr:uid="{FE88017D-A711-489B-A895-75273411F361}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:AB20">
-      <sortCondition ref="B2:B20"/>
-    </sortState>
+  <autoFilter ref="A1:CI26" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Detroit-Warren-Dearborn, MI"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>